<commit_message>
Aggiunta variable importance modelli
</commit_message>
<xml_diff>
--- a/Performance modelli.xlsx
+++ b/Performance modelli.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Davide Finati\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Davide Finati\Desktop\Universita'\Magistrale\I anno\I semestre\Machine Learning\Progetto\2019_machinelearning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AD061B93-C96D-43DC-89DF-CA9C11AB7CCE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58255DBA-B92F-4AA8-BC97-D4FE01A4DC12}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{D416BB75-78E2-4CF3-ABBA-01DCEED722E6}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="69">
   <si>
     <t>Modelli Holdout</t>
   </si>
@@ -177,9 +176,6 @@
     <t>0.874</t>
   </si>
   <si>
-    <t>42 secondi</t>
-  </si>
-  <si>
     <t>0.8246</t>
   </si>
   <si>
@@ -238,6 +234,12 @@
   </si>
   <si>
     <t>0.9046</t>
+  </si>
+  <si>
+    <t>massimizzato parametro maxdepth</t>
+  </si>
+  <si>
+    <t>22 secondi</t>
   </si>
 </sst>
 </file>
@@ -341,18 +343,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -672,7 +674,7 @@
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -685,19 +687,19 @@
     <col min="6" max="6" width="6.36328125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.453125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7.26953125" customWidth="1"/>
-    <col min="9" max="9" width="51.54296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
@@ -705,16 +707,16 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7" t="s">
+      <c r="C4" s="9"/>
+      <c r="D4" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
@@ -744,10 +746,10 @@
         <v>11</v>
       </c>
       <c r="B6" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>49</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>50</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>38</v>
@@ -767,22 +769,22 @@
         <v>9</v>
       </c>
       <c r="B7" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="D7" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="E7" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="F7" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="G7" s="5" t="s">
         <v>55</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
@@ -790,22 +792,22 @@
         <v>10</v>
       </c>
       <c r="B8" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="D8" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="E8" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="F8" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="G8" s="5" t="s">
         <v>61</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
@@ -824,22 +826,22 @@
         <v>13</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>25</v>
       </c>
       <c r="D10" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E10" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="F10" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="F10" s="5" t="s">
+      <c r="G10" s="5" t="s">
         <v>66</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
@@ -848,17 +850,17 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="7"/>
-      <c r="D13" s="9" t="s">
+      <c r="C13" s="9"/>
+      <c r="D13" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="9"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
@@ -911,62 +913,64 @@
       <c r="H15" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="I15" s="11"/>
+      <c r="I15" s="8" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A17" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B17" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="H17" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C16" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="G16" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="H16" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="I16" s="10"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A17" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="G17" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="H17" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I17" s="7"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>12</v>
       </c>
@@ -992,7 +996,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>21</v>
       </c>

</xml_diff>

<commit_message>
Aggiunte VarImp e ROC jpg
</commit_message>
<xml_diff>
--- a/Performance modelli.xlsx
+++ b/Performance modelli.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Davide Finati\Desktop\Universita'\Magistrale\I anno\I semestre\Machine Learning\Progetto\2019_machinelearning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58255DBA-B92F-4AA8-BC97-D4FE01A4DC12}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3724B75-2BF7-4888-8A3A-6D2FBC540754}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{D416BB75-78E2-4CF3-ABBA-01DCEED722E6}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="73">
   <si>
     <t>Modelli Holdout</t>
   </si>
@@ -134,18 +134,6 @@
     <t>0.9058</t>
   </si>
   <si>
-    <t>0.8318</t>
-  </si>
-  <si>
-    <t>0.87</t>
-  </si>
-  <si>
-    <t>0.92</t>
-  </si>
-  <si>
-    <t>0.8947</t>
-  </si>
-  <si>
     <t>19 secondi</t>
   </si>
   <si>
@@ -167,9 +155,6 @@
     <t>0.7764</t>
   </si>
   <si>
-    <t>0.7765</t>
-  </si>
-  <si>
     <t>0.9995</t>
   </si>
   <si>
@@ -236,10 +221,37 @@
     <t>0.9046</t>
   </si>
   <si>
-    <t>massimizzato parametro maxdepth</t>
-  </si>
-  <si>
     <t>22 secondi</t>
+  </si>
+  <si>
+    <t>0.8335</t>
+  </si>
+  <si>
+    <t>0.8507</t>
+  </si>
+  <si>
+    <t>0.9527</t>
+  </si>
+  <si>
+    <t>0.8988</t>
+  </si>
+  <si>
+    <t>TP=25016, FP=4391, FN=1241, TN=3182</t>
+  </si>
+  <si>
+    <t>0.7763</t>
+  </si>
+  <si>
+    <t>TP=26245, FP=7555, FN=12, TN=18</t>
+  </si>
+  <si>
+    <t>TP=25260, FP=4564, FN=997, TN=3009</t>
+  </si>
+  <si>
+    <t>TP=24919, FP=3859, FN=1338, TN=3714</t>
+  </si>
+  <si>
+    <t>Confusion matrix</t>
   </si>
 </sst>
 </file>
@@ -279,7 +291,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -311,22 +323,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -341,12 +342,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -673,8 +668,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93AB9987-4B35-410C-87CB-9571015600FB}">
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -687,19 +682,19 @@
     <col min="6" max="6" width="6.36328125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.453125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7.26953125" customWidth="1"/>
-    <col min="9" max="9" width="30.7265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="33.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
@@ -707,16 +702,16 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9" t="s">
+      <c r="C4" s="7"/>
+      <c r="D4" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
@@ -746,22 +741,22 @@
         <v>11</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
@@ -769,22 +764,22 @@
         <v>9</v>
       </c>
       <c r="B7" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="G7" s="5" t="s">
         <v>50</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
@@ -792,22 +787,22 @@
         <v>10</v>
       </c>
       <c r="B8" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="G8" s="5" t="s">
         <v>56</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
@@ -826,22 +821,22 @@
         <v>13</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>25</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
@@ -850,17 +845,17 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="9"/>
-      <c r="D13" s="11" t="s">
+      <c r="C13" s="7"/>
+      <c r="D13" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="11"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
@@ -887,34 +882,37 @@
       <c r="H14" s="6" t="s">
         <v>19</v>
       </c>
+      <c r="I14" s="5" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>24</v>
       </c>
       <c r="D15" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H15" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="E15" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="H15" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="I15" s="8" t="s">
-        <v>67</v>
+      <c r="I15" s="6" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
@@ -942,33 +940,38 @@
       <c r="H16" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="I16" s="6" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>43</v>
+        <v>68</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="I17" s="7"/>
+        <v>42</v>
+      </c>
+      <c r="I17" s="6" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
@@ -981,19 +984,22 @@
         <v>24</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>33</v>
+        <v>63</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>34</v>
+        <v>64</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>35</v>
+        <v>65</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>36</v>
+        <v>66</v>
       </c>
       <c r="H18" s="4" t="s">
         <v>28</v>
+      </c>
+      <c r="I18" s="6" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Ultime modifiche codice e excel
</commit_message>
<xml_diff>
--- a/Performance modelli.xlsx
+++ b/Performance modelli.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Davide Finati\Desktop\Universita'\Magistrale\I anno\I semestre\Machine Learning\Progetto\2019_machinelearning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BCFCCAD-F0B1-4606-B40F-A5537F85B245}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{856911AE-92CB-4858-975A-5F251BB39D52}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{D416BB75-78E2-4CF3-ABBA-01DCEED722E6}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="83">
   <si>
     <t>Modelli Holdout</t>
   </si>
@@ -261,6 +261,27 @@
   </si>
   <si>
     <t>TP=2990, FP=4583, FN=787, TN=25470</t>
+  </si>
+  <si>
+    <t>1 minuto</t>
+  </si>
+  <si>
+    <t>0.73 secondi</t>
+  </si>
+  <si>
+    <t>0.835</t>
+  </si>
+  <si>
+    <t>0.6688</t>
+  </si>
+  <si>
+    <t>0.5205</t>
+  </si>
+  <si>
+    <t>0.5854</t>
+  </si>
+  <si>
+    <t>TP=3942, FP=1952, FN=3631, TN=24305</t>
   </si>
 </sst>
 </file>
@@ -677,8 +698,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93AB9987-4B35-410C-87CB-9571015600FB}">
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -829,12 +850,27 @@
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
+      <c r="B9" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">

</xml_diff>